<commit_message>
edited testing script for the behavioral study
</commit_message>
<xml_diff>
--- a/data/ReverseEngineering/potential_open_source_projects.xlsx
+++ b/data/ReverseEngineering/potential_open_source_projects.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,12 +13,55 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>Repo:</t>
+  </si>
+  <si>
+    <t>Project Name</t>
+  </si>
+  <si>
+    <t>github Url</t>
+  </si>
+  <si>
+    <t>Project Language</t>
+  </si>
+  <si>
+    <t>Time tracking</t>
+  </si>
+  <si>
+    <t>XX</t>
+  </si>
+  <si>
+    <t>http://</t>
+  </si>
+  <si>
+    <t>Java, C++, etc</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>https://issues.apache.org/jira/secure/Dashboard.jspa</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -41,17 +84,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -98,7 +152,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -133,7 +187,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -341,13 +395,55 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
assign the documents to model analysis team
</commit_message>
<xml_diff>
--- a/data/ReverseEngineering/potential_open_source_projects.xlsx
+++ b/data/ReverseEngineering/potential_open_source_projects.xlsx
@@ -399,10 +399,15 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="24" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -441,9 +446,6 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>